<commit_message>
análise amplamente melhorada, muitas melhorias
</commit_message>
<xml_diff>
--- a/Filters/Filters.xlsx
+++ b/Filters/Filters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\march\Documents\MRU\Filters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CB3B39-8294-4FCA-BD96-B2E3DF03F8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66C69DA-AE1B-41FF-9E64-E0C4639A7ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="92">
   <si>
     <t>Categoria</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>Kalman + Laplace + Complementar</t>
+  </si>
+  <si>
+    <t>Filtro</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EEE06886-820B-43D3-B5FC-E94368FDA1B7}" name="Filtro Chebyshev" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{EEE06886-820B-43D3-B5FC-E94368FDA1B7}" name="Filtro" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{1CC25D36-778B-4DAB-B872-0B54426669A4}" name="Categoria" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{7D285670-3294-452A-ACAC-2EF7E6A43BD6}" name="Velocidade de Resposta" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{CEA6403E-9986-4A54-9A05-3CC5127E8BED}" name="Suavização" dataDxfId="7"/>
@@ -722,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,7 +746,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>

</xml_diff>